<commit_message>
Updated crop and user data files + modified main.py Resolved conflicts in main.py and data/crops.xlsx
</commit_message>
<xml_diff>
--- a/data/users.xlsx
+++ b/data/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,28 @@
           <t>Role</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Ayushi123</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>pokemon@123</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
tried to integrate the 2 main.py files
happy diwali
</commit_message>
<xml_diff>
--- a/data/users.xlsx
+++ b/data/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,46 +509,6 @@
       </c>
       <c r="D4" t="inlineStr"/>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>sharma</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>farmer</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>sharma</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1234567890</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>